<commit_message>
REINCORP EN ENERO Modifica 2 scripts datos correl 2a2 y spp_db.R y cuatro tablas de datos algunas de nueva creacion
</commit_message>
<xml_diff>
--- a/Data/Especies_Etiquetadas_Col_2017_NHOC_Agus.xlsx
+++ b/Data/Especies_Etiquetadas_Col_2017_NHOC_Agus.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MS_in_prep\Orquis\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MS_in_prep\Orquis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -835,10 +835,10 @@
   <dimension ref="A1:N474"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>